<commit_message>
Added Java Reflection Class's Sample project
</commit_message>
<xml_diff>
--- a/FlipkartDemo/test-data/testData.xlsx
+++ b/FlipkartDemo/test-data/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>fk001</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Sony T2 Ultra (White, 8 GB)</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -392,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -407,7 +416,7 @@
     <col min="6" max="6" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -426,8 +435,11 @@
       <c r="F1" t="s">
         <v>7</v>
       </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -446,8 +458,11 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -466,8 +481,11 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -485,6 +503,9 @@
       </c>
       <c r="F4" t="s">
         <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>